<commit_message>
Atualização automática de SANANDUVA.xlsx
</commit_message>
<xml_diff>
--- a/SANANDUVA.xlsx
+++ b/SANANDUVA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CEFD846-F23D-40D4-B12B-7069FDC0A277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1AEC74C3-30C2-405F-A2EE-6711B907532A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1182,7 +1182,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{691A9AD4-AFBB-4870-BDA9-E450F1D654B7}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{DE98C819-978B-47D6-8FDF-0F7FF8CB0C76}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1212,10 +1212,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B56194FD-235B-4F54-AAB0-5B06887E20FB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{052F78D4-1F38-445E-BB85-5C018EDA7152}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1253,7 +1253,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{895F1537-902C-42BC-A370-909939F0C211}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7C55A4D-F8D1-4A4F-A56E-42DF60BF3F2B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1316,7 +1316,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A3A51AF-E38E-49C7-99D8-B93FABC97CF4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8344B7D-D405-4B93-97E5-4EE6437D021E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1335,7 +1335,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C19D19F7-3C6F-41DE-C58D-A20327354588}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39830B87-7194-3DDA-9BCD-B0119D94DA49}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1384,7 +1384,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B3F00F0-4966-14FD-0945-EC5AC1674AA7}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F154160-505F-5BEB-356D-8BF79E055EC8}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1403,7 +1403,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D30E7CF-8621-8855-DA49-62B6F7B0EAF8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A434A2E4-578B-8694-4B07-BE10394D7C8E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1434,7 +1434,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C8F9E52-C87C-E99C-60C3-FF125E08DE48}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A596BCA8-A53C-A6EC-36AB-1CEE00438160}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1465,7 +1465,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22DE4C0D-881D-DEA8-D66F-95139881C66E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94E75EAE-5006-9A7A-65A0-BFD7D51F9F12}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1508,7 +1508,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DCBBEE4-A2EA-4113-A0EB-E40416CFCDA7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82A4E819-F2A8-4635-B166-7B82566CB595}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1546,7 +1546,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8BD457B-3E7F-4680-B1F8-A0DF3C341EA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1388F636-55D7-42B2-9F22-DC7673937D82}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1589,7 +1589,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7303F34-EED1-4D82-8B89-30996D6BD4AB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98A4CAF7-5905-4873-881C-BFA78566096C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1902,7 +1902,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{621DEE77-4AA1-49FD-8F8B-76D32DD45B02}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A1B0540-8235-4535-A196-CB25E17BCCBA}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>